<commit_message>
Assign 'valid min' and 'valid max' in files
</commit_message>
<xml_diff>
--- a/specific_variables/aerosol-concentration.xlsx
+++ b/specific_variables/aerosol-concentration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/specific_variables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DB42F9-82A5-464B-84C0-D9EBCEA5A2F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6178298F-6A23-7447-82B8-EE39893BE3E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33960" yWindow="-3120" windowWidth="22180" windowHeight="19020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Variable</t>
   </si>
@@ -64,12 +64,6 @@
     <t>_FillValue</t>
   </si>
   <si>
-    <t>valid_min</t>
-  </si>
-  <si>
-    <t>valid_max</t>
-  </si>
-  <si>
     <t>coordinates</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
 good_data, 
 suspect_data_not_wind_direction_filtered 
   </t>
-  </si>
-  <si>
-    <t>&lt;derived&gt;</t>
   </si>
 </sst>
 </file>
@@ -157,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -179,7 +170,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -510,7 +500,7 @@
   <dimension ref="A1:W997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="A17:C17"/>
+      <selection activeCell="C10" sqref="A9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -554,7 +544,7 @@
       <c r="W1" s="4"/>
     </row>
     <row r="2" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3"/>
@@ -619,93 +609,81 @@
       <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>25</v>
+      <c r="C9" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>25</v>
-      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="10"/>
     </row>
     <row r="11" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="10"/>
+    </row>
+    <row r="12" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="11"/>
-    </row>
     <row r="13" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="3" t="s">
-        <v>18</v>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3" t="s">
+        <v>7</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="11"/>
+      <c r="C13" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>19</v>
+      <c r="C14" s="6">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
-        <v>2</v>
+      <c r="B16" s="11" t="s">
+        <v>19</v>
       </c>
-      <c r="C16" s="6">
-        <v>1</v>
+      <c r="C16" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3"/>
-      <c r="B17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="3"/>
-      <c r="B18" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4" t="s">
+      <c r="C17" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>24</v>
-      </c>
+    </row>
+    <row r="18" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C20" s="6"/>
@@ -3629,12 +3607,8 @@
     <row r="993" spans="3:3" ht="13" x14ac:dyDescent="0.15">
       <c r="C993" s="6"/>
     </row>
-    <row r="994" spans="3:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="C994" s="6"/>
-    </row>
-    <row r="995" spans="3:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="C995" s="6"/>
-    </row>
+    <row r="994" spans="3:3" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="995" spans="3:3" ht="13" x14ac:dyDescent="0.15"/>
     <row r="996" spans="3:3" ht="13" x14ac:dyDescent="0.15"/>
     <row r="997" spans="3:3" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>

</xml_diff>

<commit_message>
Added valid min and max to aerosol specific variables
</commit_message>
<xml_diff>
--- a/specific_variables/aerosol-concentration.xlsx
+++ b/specific_variables/aerosol-concentration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/specific_variables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001191F4-7B15-054C-B750-AD561CE612DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6E63BB-224C-2147-9FAD-EAF83BFFCDEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29800" yWindow="-2700" windowWidth="22180" windowHeight="19020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Variable</t>
   </si>
@@ -94,12 +94,27 @@
   <si>
     <t>0b,1b, 2b, 3b, 4b</t>
   </si>
+  <si>
+    <t>valid_min</t>
+  </si>
+  <si>
+    <t>&lt;derived from file&gt;</t>
+  </si>
+  <si>
+    <t>valid_max</t>
+  </si>
+  <si>
+    <t>cell_methods</t>
+  </si>
+  <si>
+    <t>time: median</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -128,6 +143,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -149,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -181,6 +205,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -502,7 +534,7 @@
   <dimension ref="A1:W997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -607,89 +639,113 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3" t="s">
-        <v>14</v>
+      <c r="A9" s="14"/>
+      <c r="B9" s="14" t="s">
+        <v>23</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>15</v>
+      <c r="C9" s="15" t="s">
+        <v>24</v>
       </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="10"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
     </row>
     <row r="11" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="3" t="s">
-        <v>16</v>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16" t="s">
+        <v>26</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="10"/>
+      <c r="C11" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="14"/>
     </row>
     <row r="12" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>17</v>
+      <c r="C12" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
-      <c r="B13" s="3" t="s">
-        <v>7</v>
+      <c r="B13" s="3"/>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="3" t="s">
+        <v>16</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="6">
-        <v>1</v>
-      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="10"/>
     </row>
     <row r="15" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="3"/>
-      <c r="B16" s="12" t="s">
+    <row r="19" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="3"/>
+      <c r="B19" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C19" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="3"/>
-      <c r="B17" s="4" t="s">
+    <row r="20" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C20" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C19" s="6"/>
-    </row>
-    <row r="20" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C20" s="6"/>
-    </row>
     <row r="21" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C21" s="6"/>
     </row>
@@ -3609,9 +3665,15 @@
     <row r="993" spans="3:3" ht="13" x14ac:dyDescent="0.15">
       <c r="C993" s="6"/>
     </row>
-    <row r="994" spans="3:3" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="995" spans="3:3" ht="13" x14ac:dyDescent="0.15"/>
-    <row r="996" spans="3:3" ht="13" x14ac:dyDescent="0.15"/>
+    <row r="994" spans="3:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="C994" s="6"/>
+    </row>
+    <row r="995" spans="3:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="C995" s="6"/>
+    </row>
+    <row r="996" spans="3:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="C996" s="6"/>
+    </row>
     <row r="997" spans="3:3" ht="13" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Netcdf parser for CPC updated
</commit_message>
<xml_diff>
--- a/specific_variables/aerosol-concentration.xlsx
+++ b/specific_variables/aerosol-concentration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/specific_variables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6E63BB-224C-2147-9FAD-EAF83BFFCDEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73699BC-A34E-9442-8032-57B6EFAAE7AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29800" yWindow="-2700" windowWidth="22180" windowHeight="19020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="500" yWindow="460" windowWidth="20460" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variables-specific" sheetId="2" r:id="rId1"/>
@@ -85,13 +85,6 @@
     <t>flag_meanings</t>
   </si>
   <si>
-    <t>not_used
-good_data 
-bad_data_station_pollution_advecting_past_instrument
-bad_data_unspecified_instrument_error
-suspect_data_no_met_data_available_to_qc_for_station_pollution</t>
-  </si>
-  <si>
     <t>0b,1b, 2b, 3b, 4b</t>
   </si>
   <si>
@@ -108,6 +101,12 @@
   </si>
   <si>
     <t>time: median</t>
+  </si>
+  <si>
+    <t>not_used
+good_data 
+bad_data_station_pollution_advecting_past_instrument
+suspect_data_no_met_data_available_to_qc_for_station_pollution</t>
   </si>
 </sst>
 </file>
@@ -534,7 +533,7 @@
   <dimension ref="A1:W997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -641,10 +640,10 @@
     <row r="9" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14"/>
       <c r="B9" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -652,10 +651,10 @@
     <row r="10" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="14"/>
       <c r="B10" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
@@ -663,10 +662,10 @@
     <row r="11" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="16"/>
       <c r="B11" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="14"/>
@@ -734,7 +733,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -743,7 +742,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Aerosol size distribution netcdf parsing
</commit_message>
<xml_diff>
--- a/specific_variables/aerosol-concentration.xlsx
+++ b/specific_variables/aerosol-concentration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/specific_variables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73699BC-A34E-9442-8032-57B6EFAAE7AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A8E424-15FE-5647-897C-E3BFEE4F9B20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="460" windowWidth="20460" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,9 +85,6 @@
     <t>flag_meanings</t>
   </si>
   <si>
-    <t>0b,1b, 2b, 3b, 4b</t>
-  </si>
-  <si>
     <t>valid_min</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
 good_data 
 bad_data_station_pollution_advecting_past_instrument
 suspect_data_no_met_data_available_to_qc_for_station_pollution</t>
+  </si>
+  <si>
+    <t>0b,1b, 2b, 3b</t>
   </si>
 </sst>
 </file>
@@ -640,10 +640,10 @@
     <row r="9" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="14"/>
       <c r="B9" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -651,10 +651,10 @@
     <row r="10" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="14"/>
       <c r="B10" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
@@ -662,10 +662,10 @@
     <row r="11" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="16"/>
       <c r="B11" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="14"/>
@@ -733,7 +733,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -742,7 +742,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Updated qc flag format
</commit_message>
<xml_diff>
--- a/specific_variables/aerosol-concentration.xlsx
+++ b/specific_variables/aerosol-concentration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/specific_variables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A8E424-15FE-5647-897C-E3BFEE4F9B20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F42CF5-8279-3E4B-8EA2-DC58C7F8DB05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="500" yWindow="460" windowWidth="20460" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,13 +100,10 @@
     <t>time: median</t>
   </si>
   <si>
-    <t>not_used
-good_data 
-bad_data_station_pollution_advecting_past_instrument
-suspect_data_no_met_data_available_to_qc_for_station_pollution</t>
+    <t>0, 1, 2, 3</t>
   </si>
   <si>
-    <t>0b,1b, 2b, 3b</t>
+    <t>not_used good_data bad_data_station_pollution_advecting_past_instrument suspect_data_no_met_data_available_to_qc_for_station_pollution</t>
   </si>
 </sst>
 </file>
@@ -733,7 +730,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -742,7 +739,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Update aerosol codes to qc for technicians logs
</commit_message>
<xml_diff>
--- a/specific_variables/aerosol-concentration.xlsx
+++ b/specific_variables/aerosol-concentration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/specific_variables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F42CF5-8279-3E4B-8EA2-DC58C7F8DB05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D4431A-06DF-6E43-8A8F-7B5137899435}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="460" windowWidth="20460" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35500" yWindow="-1820" windowWidth="28940" windowHeight="17980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variables-specific" sheetId="2" r:id="rId1"/>
@@ -100,10 +100,10 @@
     <t>time: median</t>
   </si>
   <si>
-    <t>0, 1, 2, 3</t>
+    <t>not_used good_data bad_data_station_pollution_advecting_past_instrument suspect_data_no_met_data_available_to_qc_for_station_pollution bad_data_technician_log</t>
   </si>
   <si>
-    <t>not_used good_data bad_data_station_pollution_advecting_past_instrument suspect_data_no_met_data_available_to_qc_for_station_pollution</t>
+    <t>0, 1, 2, 3, 4</t>
   </si>
 </sst>
 </file>
@@ -730,7 +730,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -739,7 +739,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>